<commit_message>
definities toegevoegd en aangepast
</commit_message>
<xml_diff>
--- a/BGGZ/Documentatie/bggz bestanden definities.xlsx
+++ b/BGGZ/Documentatie/bggz bestanden definities.xlsx
@@ -2273,7 +2273,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="60.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.1"/>
@@ -2710,10 +2710,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.88"/>

</xml_diff>